<commit_message>
Update parac hakkında dizi bazlı aramalar.xlsx
</commit_message>
<xml_diff>
--- a/parac hakkında dizi bazlı aramalar.xlsx
+++ b/parac hakkında dizi bazlı aramalar.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28512"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBCA7089-2076-40A9-9F8A-ED46FAF8B01F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C23593A2-345F-4A09-B128-4FD220200A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>p</t>
   </si>
@@ -52,6 +52,69 @@
   </si>
   <si>
     <t>max/4</t>
+  </si>
+  <si>
+    <t>Max nereden elde ediliyor?</t>
+  </si>
+  <si>
+    <t>a1+a1</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>a2+a2</t>
+  </si>
+  <si>
+    <t>a3+a3</t>
+  </si>
+  <si>
+    <t>Son-1</t>
+  </si>
+  <si>
+    <t>a4+a4</t>
+  </si>
+  <si>
+    <t>a4+a3</t>
+  </si>
+  <si>
+    <t>Son,Son-1</t>
+  </si>
+  <si>
+    <t>a5+a4</t>
+  </si>
+  <si>
+    <t>a6+a5</t>
+  </si>
+  <si>
+    <t>a6+a6</t>
+  </si>
+  <si>
+    <t>a7+a6</t>
+  </si>
+  <si>
+    <t>a7+a5</t>
+  </si>
+  <si>
+    <t>Son,Son-2</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>a7+a7</t>
+  </si>
+  <si>
+    <t>Son-2</t>
+  </si>
+  <si>
+    <t>Son-1,Son-2</t>
+  </si>
+  <si>
+    <t>a8+a8</t>
+  </si>
+  <si>
+    <t>Max/4 ile kıyaslama</t>
   </si>
   <si>
     <t>farklar</t>
@@ -85,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,8 +185,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -159,22 +228,104 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:AI63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L34" workbookViewId="0">
-      <selection activeCell="Y51" sqref="Y51"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24:Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -520,7 +671,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:19">
+    <row r="2" spans="3:27">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,18 +693,26 @@
       <c r="S2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="3:19">
+      <c r="W2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:27">
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <f>E3/D3</f>
         <v>2</v>
       </c>
@@ -567,30 +726,44 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" s="1">
+      <c r="P3" s="12">
         <f>_xlfn.STDEV.P(H3:O3)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="1">
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12">
         <f>E3/2</f>
         <v>1</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="12">
         <f>E3/4</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="3:19">
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:27">
       <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <f>E4/D4</f>
         <v>3</v>
       </c>
@@ -618,18 +791,28 @@
         <f t="shared" ref="S4:S22" si="1">E4/4</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="5" spans="3:19">
+      <c r="W4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:27">
       <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>10</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <f>E5/D5</f>
         <v>3.3333333333333335</v>
       </c>
@@ -647,30 +830,44 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="1">
+      <c r="P5" s="12">
         <f>_xlfn.STDEV.P(H5:O5)</f>
         <v>1.247219128924647</v>
       </c>
-      <c r="R5" s="1">
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="12">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="6" spans="3:19">
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:27">
       <c r="C6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>3</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>10</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <f>E6/D6</f>
         <v>3.3333333333333335</v>
       </c>
@@ -700,18 +897,28 @@
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="7" spans="3:19">
+      <c r="W6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:27">
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>16</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <f>E7/D7</f>
         <v>4</v>
       </c>
@@ -731,30 +938,44 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="1">
+      <c r="P7" s="12">
         <f>_xlfn.STDEV.P(H7:O7)</f>
         <v>4.8476798574163293</v>
       </c>
-      <c r="R7" s="1">
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="12">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="3:19">
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:27">
       <c r="C8" s="1">
         <v>6</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>4</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>16</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4">
         <f>E8/D8</f>
         <v>4</v>
       </c>
@@ -786,18 +1007,28 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="3:19">
+      <c r="W8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:27">
       <c r="C9" s="1">
         <v>7</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>4</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>16</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="4">
         <f>E9/D9</f>
         <v>4</v>
       </c>
@@ -817,30 +1048,44 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="1">
+      <c r="P9" s="12">
         <f>_xlfn.STDEV.P(H9:O9)</f>
         <v>1.8027756377319946</v>
       </c>
-      <c r="R9" s="1">
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" s="12">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="3:19">
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:27">
       <c r="C10" s="1">
         <v>8</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>5</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>24</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="4">
         <f>E10/D10</f>
         <v>4.8</v>
       </c>
@@ -874,18 +1119,28 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="3:19">
+      <c r="W10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y10" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:27">
       <c r="C11" s="1">
         <v>9</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>6</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>32</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="4">
         <f t="shared" ref="F11:F19" si="2">E11/D11</f>
         <v>5.333333333333333</v>
       </c>
@@ -909,30 +1164,44 @@
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="1">
+      <c r="P11" s="12">
         <f>_xlfn.STDEV.P(H11:O11)</f>
         <v>4.4221663871405337</v>
       </c>
-      <c r="R11" s="1">
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="12">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="3:19">
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="3:27">
       <c r="C12" s="1">
         <v>10</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>6</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>32</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="4">
         <f t="shared" si="2"/>
         <v>5.333333333333333</v>
       </c>
@@ -968,18 +1237,28 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="3:19">
+      <c r="W12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="3:27">
       <c r="C13" s="1">
         <v>11</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>7</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>40</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="4">
         <f t="shared" si="2"/>
         <v>5.7142857142857144</v>
       </c>
@@ -1005,30 +1284,44 @@
         <v>21</v>
       </c>
       <c r="O13" s="5"/>
-      <c r="P13" s="1">
+      <c r="P13" s="12">
         <f>_xlfn.STDEV.P(H13:O13)</f>
         <v>5.9039938056490922</v>
       </c>
-      <c r="R13" s="1">
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="S13" s="1">
+      <c r="S13" s="12">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="3:19">
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:27">
       <c r="C14" s="1">
         <v>12</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>7</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>40</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="4">
         <f t="shared" si="2"/>
         <v>5.7142857142857144</v>
       </c>
@@ -1066,18 +1359,28 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="3:19">
+      <c r="W14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="3:27">
       <c r="C15" s="1">
         <v>13</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>7</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>40</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="4">
         <f t="shared" si="2"/>
         <v>5.7142857142857144</v>
       </c>
@@ -1103,30 +1406,44 @@
         <v>21</v>
       </c>
       <c r="O15" s="5"/>
-      <c r="P15" s="1">
+      <c r="P15" s="12">
         <f>_xlfn.STDEV.P(H15:O15)</f>
         <v>5.7817446699565895</v>
       </c>
-      <c r="R15" s="1">
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="S15" s="1">
+      <c r="S15" s="12">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="3:19">
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y15" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="3:27">
       <c r="C16" s="1">
         <v>14</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>7</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>40</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="2"/>
         <v>5.7142857142857144</v>
       </c>
@@ -1164,18 +1481,28 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="W16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="17">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="3:35">
       <c r="C17" s="1">
         <v>15</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>7</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>40</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="4">
         <f t="shared" si="2"/>
         <v>5.7142857142857144</v>
       </c>
@@ -1201,30 +1528,44 @@
         <v>40</v>
       </c>
       <c r="O17" s="5"/>
-      <c r="P17" s="1">
+      <c r="P17" s="12">
         <f>_xlfn.STDEV.P(H17:O17)</f>
         <v>10.23200261683999</v>
       </c>
-      <c r="R17" s="1">
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="S17" s="1">
+      <c r="S17" s="12">
         <f t="shared" si="1"/>
         <v>10</v>
+      </c>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="17">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="3:35">
       <c r="C18" s="1">
         <v>16</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>7</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>40</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="4">
         <f t="shared" si="2"/>
         <v>5.7142857142857144</v>
       </c>
@@ -1262,18 +1603,28 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="W18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="17">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="3:35">
       <c r="C19" s="1">
         <v>17</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>7</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>40</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="4">
         <f t="shared" si="2"/>
         <v>5.7142857142857144</v>
       </c>
@@ -1299,30 +1650,44 @@
         <v>40</v>
       </c>
       <c r="O19" s="5"/>
-      <c r="P19" s="1">
+      <c r="P19" s="12">
         <f>_xlfn.STDEV.P(H19:O19)</f>
         <v>10.00612057590712</v>
       </c>
-      <c r="R19" s="1">
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="S19" s="1">
+      <c r="S19" s="12">
         <f t="shared" si="1"/>
         <v>10</v>
+      </c>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="17">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="3:35">
       <c r="C20" s="1">
         <v>18</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>8</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>52</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="4">
         <f>E20/D20</f>
         <v>6.5</v>
       </c>
@@ -1362,18 +1727,28 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="W20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y20" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="13">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="3:35">
       <c r="C21" s="1">
         <v>19</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>8</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>52</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="4">
         <f>E21/D21</f>
         <v>6.5</v>
       </c>
@@ -1401,30 +1776,44 @@
       <c r="O21" s="5">
         <v>55</v>
       </c>
-      <c r="P21" s="1">
+      <c r="P21" s="12">
         <f>_xlfn.STDEV.P(H21:O21)</f>
         <v>14.291059267947915</v>
       </c>
-      <c r="R21" s="1">
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="S21" s="1">
+      <c r="S21" s="12">
         <f t="shared" si="1"/>
         <v>13</v>
+      </c>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z21" s="14"/>
+      <c r="AA21" s="13">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="3:35">
       <c r="C22" s="1">
         <v>20</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>8</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>52</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="4">
         <f>E22/D22</f>
         <v>6.5</v>
       </c>
@@ -1464,13 +1853,30 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="W22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y22" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:35">
+      <c r="O24" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
     </row>
     <row r="25" spans="3:35">
       <c r="G25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
@@ -1480,75 +1886,75 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V25" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="W25" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="X25" s="9"/>
-      <c r="Y25" s="9"/>
-      <c r="Z25" s="9"/>
-      <c r="AA25" s="9"/>
-      <c r="AB25" s="9"/>
-      <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
-      <c r="AE25" s="9"/>
-      <c r="AF25" s="9"/>
-      <c r="AG25" s="9"/>
-      <c r="AH25" s="9"/>
-      <c r="AI25" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="V25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AD25" s="7"/>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7"/>
     </row>
     <row r="26" spans="3:35">
       <c r="F26" s="1">
         <v>2</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>2</v>
       </c>
-      <c r="H26" s="4">
-        <v>1</v>
-      </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
       <c r="O26" s="6"/>
       <c r="P26" s="1">
         <f>_xlfn.STDEV.P(H26:O26)</f>
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="b">
-        <f t="shared" ref="Q26:Q44" si="3">IF(S26&gt;P26,TRUE)</f>
+        <f>IF(S26&gt;P26,TRUE)</f>
         <v>1</v>
       </c>
       <c r="S26" s="1">
-        <f t="shared" ref="S26:S44" si="4">S4</f>
+        <f t="shared" ref="S26:S44" si="3">S4</f>
         <v>1.5</v>
       </c>
       <c r="T26" s="1">
         <f>(G26*G26+G26)/4</f>
         <v>1.5</v>
       </c>
-      <c r="V26" s="9">
+      <c r="V26" s="7">
         <f>SUM(H26:N26)</f>
         <v>1</v>
       </c>
-      <c r="W26" s="9">
+      <c r="W26" s="7">
         <f>V26/(G26-1)</f>
         <v>1</v>
       </c>
-      <c r="X26" s="9"/>
+      <c r="X26" s="7"/>
       <c r="Y26" s="8">
         <f>H26-W26</f>
         <v>0</v>
@@ -1559,55 +1965,55 @@
       <c r="AC26" s="8"/>
       <c r="AD26" s="8"/>
       <c r="AE26" s="8"/>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="9"/>
-      <c r="AH26" s="9"/>
-      <c r="AI26" s="9"/>
+      <c r="AF26" s="7"/>
+      <c r="AG26" s="7"/>
+      <c r="AH26" s="7"/>
+      <c r="AI26" s="7"/>
     </row>
     <row r="27" spans="3:35">
       <c r="F27" s="1">
         <v>3</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>3</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <v>2</v>
       </c>
-      <c r="I27" s="4">
-        <v>1</v>
-      </c>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
       <c r="O27" s="6"/>
       <c r="P27" s="1">
-        <f t="shared" ref="P23:P63" si="5">_xlfn.STDEV.P(H27:O27)</f>
+        <f t="shared" ref="P23:P63" si="4">_xlfn.STDEV.P(H27:O27)</f>
         <v>0.5</v>
       </c>
       <c r="Q27" s="1" t="b">
+        <f t="shared" ref="Q26:Q44" si="5">IF(S27&gt;P27,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="S27" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S27" s="1">
-        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
       <c r="T27" s="1">
         <f t="shared" ref="T27:T44" si="6">(G27*G27+G27)/4</f>
         <v>3</v>
       </c>
-      <c r="V27" s="9">
+      <c r="V27" s="7">
         <f t="shared" ref="V27:V44" si="7">SUM(H27:N27)</f>
         <v>3</v>
       </c>
-      <c r="W27" s="9">
+      <c r="W27" s="7">
         <f t="shared" ref="W27:W44" si="8">V27/(G27-1)</f>
         <v>1.5</v>
       </c>
-      <c r="X27" s="9"/>
+      <c r="X27" s="7"/>
       <c r="Y27" s="8">
         <f>H27-W27</f>
         <v>0.5</v>
@@ -1621,55 +2027,55 @@
       <c r="AC27" s="8"/>
       <c r="AD27" s="8"/>
       <c r="AE27" s="8"/>
-      <c r="AF27" s="9"/>
-      <c r="AG27" s="9"/>
-      <c r="AH27" s="9"/>
-      <c r="AI27" s="9"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
     </row>
     <row r="28" spans="3:35">
       <c r="F28" s="1">
         <v>4</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>3</v>
       </c>
-      <c r="H28" s="4">
-        <v>1</v>
-      </c>
-      <c r="I28" s="4">
-        <v>1</v>
-      </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
       <c r="O28" s="6"/>
       <c r="P28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q28" s="1" t="b">
+        <f>IF(S28&gt;P28,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="S28" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S28" s="1">
-        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
       <c r="T28" s="1">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="V28" s="9">
+      <c r="V28" s="7">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="W28" s="9">
+      <c r="W28" s="7">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="X28" s="9"/>
+      <c r="X28" s="7"/>
       <c r="Y28" s="8">
         <f>H28-W28</f>
         <v>0</v>
@@ -1683,57 +2089,57 @@
       <c r="AC28" s="8"/>
       <c r="AD28" s="8"/>
       <c r="AE28" s="8"/>
-      <c r="AF28" s="9"/>
-      <c r="AG28" s="9"/>
-      <c r="AH28" s="9"/>
-      <c r="AI28" s="9"/>
+      <c r="AF28" s="7"/>
+      <c r="AG28" s="7"/>
+      <c r="AH28" s="7"/>
+      <c r="AI28" s="7"/>
     </row>
     <row r="29" spans="3:35">
       <c r="F29" s="1">
         <v>5</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>4</v>
       </c>
-      <c r="H29" s="4">
-        <v>1</v>
-      </c>
-      <c r="I29" s="4">
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3">
         <v>6</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="3">
         <v>5</v>
       </c>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
       <c r="O29" s="6"/>
       <c r="P29" s="1">
         <f>_xlfn.STDEV.P(H29:O29)</f>
         <v>2.1602468994692869</v>
       </c>
       <c r="Q29" s="1" t="b">
+        <f>IF(S29&gt;P29,TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="S29" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S29" s="1">
-        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="T29" s="1">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="V29" s="9">
+      <c r="V29" s="7">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="W29" s="9">
+      <c r="W29" s="7">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="X29" s="9"/>
+      <c r="X29" s="7"/>
       <c r="Y29" s="8">
         <f>H29-W29</f>
         <v>-3</v>
@@ -1750,57 +2156,57 @@
       <c r="AC29" s="8"/>
       <c r="AD29" s="8"/>
       <c r="AE29" s="8"/>
-      <c r="AF29" s="9"/>
-      <c r="AG29" s="9"/>
-      <c r="AH29" s="9"/>
-      <c r="AI29" s="9"/>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="7"/>
+      <c r="AH29" s="7"/>
+      <c r="AI29" s="7"/>
     </row>
     <row r="30" spans="3:35">
       <c r="F30" s="1">
         <v>6</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <v>4</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="3">
         <v>3</v>
       </c>
-      <c r="I30" s="4">
-        <v>1</v>
-      </c>
-      <c r="J30" s="4">
-        <v>1</v>
-      </c>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
+      <c r="I30" s="3">
+        <v>1</v>
+      </c>
+      <c r="J30" s="3">
+        <v>1</v>
+      </c>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
       <c r="O30" s="6"/>
       <c r="P30" s="1">
+        <f t="shared" si="4"/>
+        <v>0.94280904158206336</v>
+      </c>
+      <c r="Q30" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>0.94280904158206336</v>
-      </c>
-      <c r="Q30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S30" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S30" s="1">
-        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="T30" s="1">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="V30" s="9">
+      <c r="V30" s="7">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="W30" s="9">
+      <c r="W30" s="7">
         <f t="shared" si="8"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="X30" s="9"/>
+      <c r="X30" s="7"/>
       <c r="Y30" s="8">
         <f>H30-W30</f>
         <v>1.3333333333333333</v>
@@ -1817,57 +2223,57 @@
       <c r="AC30" s="8"/>
       <c r="AD30" s="8"/>
       <c r="AE30" s="8"/>
-      <c r="AF30" s="9"/>
-      <c r="AG30" s="9"/>
-      <c r="AH30" s="9"/>
-      <c r="AI30" s="9"/>
+      <c r="AF30" s="7"/>
+      <c r="AG30" s="7"/>
+      <c r="AH30" s="7"/>
+      <c r="AI30" s="7"/>
     </row>
     <row r="31" spans="3:35">
       <c r="F31" s="1">
         <v>7</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <v>4</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="3">
         <v>2</v>
       </c>
-      <c r="I31" s="4">
-        <v>1</v>
-      </c>
-      <c r="J31" s="4">
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3">
         <v>2</v>
       </c>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
       <c r="O31" s="6"/>
       <c r="P31" s="1">
+        <f t="shared" si="4"/>
+        <v>0.47140452079103168</v>
+      </c>
+      <c r="Q31" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>0.47140452079103168</v>
-      </c>
-      <c r="Q31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S31" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S31" s="1">
-        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="T31" s="1">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="V31" s="9">
+      <c r="V31" s="7">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="W31" s="9">
+      <c r="W31" s="7">
         <f t="shared" si="8"/>
         <v>1.6666666666666667</v>
       </c>
-      <c r="X31" s="9"/>
+      <c r="X31" s="7"/>
       <c r="Y31" s="8">
         <f>H31-W31</f>
         <v>0.33333333333333326</v>
@@ -1884,63 +2290,63 @@
       <c r="AC31" s="8"/>
       <c r="AD31" s="8"/>
       <c r="AE31" s="8"/>
-      <c r="AF31" s="9"/>
-      <c r="AG31" s="9"/>
-      <c r="AH31" s="9"/>
-      <c r="AI31" s="9"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
     </row>
     <row r="32" spans="3:35">
       <c r="F32" s="1">
         <v>8</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="2">
         <v>5</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32" s="3">
         <f>I10-H10</f>
         <v>4</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="3">
         <f>J10-I10</f>
         <v>2</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="3">
         <f>K10-J10</f>
         <v>1</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K32" s="3">
         <f>L10-K10</f>
         <v>2</v>
       </c>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
       <c r="O32" s="6"/>
       <c r="P32" s="1">
+        <f t="shared" si="4"/>
+        <v>1.0897247358851685</v>
+      </c>
+      <c r="Q32" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>1.0897247358851685</v>
-      </c>
-      <c r="Q32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S32" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S32" s="1">
-        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="T32" s="1">
         <f t="shared" si="6"/>
         <v>7.5</v>
       </c>
-      <c r="V32" s="9">
+      <c r="V32" s="7">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="W32" s="9">
+      <c r="W32" s="7">
         <f t="shared" si="8"/>
         <v>2.25</v>
       </c>
-      <c r="X32" s="9"/>
+      <c r="X32" s="7"/>
       <c r="Y32" s="8">
         <f t="shared" ref="Y30:AC44" si="10">H32-W32</f>
         <v>1.75</v>
@@ -1960,66 +2366,66 @@
       <c r="AC32" s="8"/>
       <c r="AD32" s="8"/>
       <c r="AE32" s="8"/>
-      <c r="AF32" s="9"/>
-      <c r="AG32" s="9"/>
-      <c r="AH32" s="9"/>
-      <c r="AI32" s="9"/>
+      <c r="AF32" s="7"/>
+      <c r="AG32" s="7"/>
+      <c r="AH32" s="7"/>
+      <c r="AI32" s="7"/>
     </row>
     <row r="33" spans="6:35">
       <c r="F33" s="1">
         <v>9</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="2">
         <v>6</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="3">
         <f>I11-H11</f>
         <v>4</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="3">
         <f>J11-I11</f>
         <v>4</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33" s="3">
         <f>K11-J11</f>
         <v>2</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K33" s="3">
         <f>L11-K11</f>
         <v>1</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="3">
         <f>M11-L11</f>
         <v>2</v>
       </c>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
       <c r="O33" s="6"/>
       <c r="P33" s="1">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="Q33" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>1.2</v>
-      </c>
-      <c r="Q33" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S33" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S33" s="1">
-        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="T33" s="1">
         <f t="shared" si="6"/>
         <v>10.5</v>
       </c>
-      <c r="V33" s="9">
+      <c r="V33" s="7">
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
-      <c r="W33" s="9">
+      <c r="W33" s="7">
         <f t="shared" si="8"/>
         <v>2.6</v>
       </c>
-      <c r="X33" s="9"/>
+      <c r="X33" s="7"/>
       <c r="Y33" s="8">
         <f t="shared" si="10"/>
         <v>1.4</v>
@@ -2042,66 +2448,66 @@
       </c>
       <c r="AD33" s="8"/>
       <c r="AE33" s="8"/>
-      <c r="AF33" s="9"/>
-      <c r="AG33" s="9"/>
-      <c r="AH33" s="9"/>
-      <c r="AI33" s="9"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
     </row>
     <row r="34" spans="6:35">
       <c r="F34" s="1">
         <v>10</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="2">
         <v>6</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="3">
         <f t="shared" ref="H34:L34" si="13">I12-H12</f>
         <v>2</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34" s="3">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="3">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="3">
         <f t="shared" si="13"/>
         <v>2</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34" s="3">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
       <c r="O34" s="6"/>
       <c r="P34" s="1">
+        <f t="shared" si="4"/>
+        <v>1.4696938456699069</v>
+      </c>
+      <c r="Q34" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>1.4696938456699069</v>
-      </c>
-      <c r="Q34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S34" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S34" s="1">
-        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="T34" s="1">
         <f t="shared" si="6"/>
         <v>10.5</v>
       </c>
-      <c r="V34" s="9">
+      <c r="V34" s="7">
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="W34" s="9">
+      <c r="W34" s="7">
         <f t="shared" si="8"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="X34" s="9"/>
+      <c r="X34" s="7"/>
       <c r="Y34" s="8">
         <f t="shared" si="10"/>
         <v>-0.20000000000000018</v>
@@ -2124,69 +2530,69 @@
       </c>
       <c r="AD34" s="8"/>
       <c r="AE34" s="8"/>
-      <c r="AF34" s="9"/>
-      <c r="AG34" s="9"/>
-      <c r="AH34" s="9"/>
-      <c r="AI34" s="9"/>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="7"/>
+      <c r="AI34" s="7"/>
     </row>
     <row r="35" spans="6:35">
       <c r="F35" s="1">
         <v>11</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="2">
         <v>7</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="3">
         <f t="shared" ref="H35:L35" si="15">I13-H13</f>
         <v>9</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="3">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="3">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K35" s="3">
         <f t="shared" si="15"/>
         <v>4</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="3">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35" s="3">
         <f t="shared" ref="M35:N35" si="16">N13-M13</f>
         <v>2</v>
       </c>
-      <c r="N35" s="4"/>
+      <c r="N35" s="3"/>
       <c r="O35" s="6"/>
       <c r="P35" s="1">
+        <f t="shared" si="4"/>
+        <v>2.7938424357067015</v>
+      </c>
+      <c r="Q35" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>2.7938424357067015</v>
-      </c>
-      <c r="Q35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S35" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S35" s="1">
-        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="T35" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="V35" s="9">
+      <c r="V35" s="7">
         <f t="shared" si="7"/>
         <v>19</v>
       </c>
-      <c r="W35" s="9">
+      <c r="W35" s="7">
         <f t="shared" si="8"/>
         <v>3.1666666666666665</v>
       </c>
-      <c r="X35" s="9"/>
+      <c r="X35" s="7"/>
       <c r="Y35" s="8">
         <f t="shared" si="10"/>
         <v>5.8333333333333339</v>
@@ -2212,69 +2618,69 @@
         <v>-1.1666666666666665</v>
       </c>
       <c r="AE35" s="8"/>
-      <c r="AF35" s="9"/>
-      <c r="AG35" s="9"/>
-      <c r="AH35" s="9"/>
-      <c r="AI35" s="9"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
     </row>
     <row r="36" spans="6:35">
       <c r="F36" s="1">
         <v>12</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="2">
         <v>7</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <f t="shared" ref="H36:L36" si="17">I14-H14</f>
         <v>11</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="3">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="3">
         <f t="shared" si="17"/>
         <v>2</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36" s="3">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36" s="3">
         <f t="shared" si="17"/>
         <v>5</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36" s="3">
         <f t="shared" ref="M36:N36" si="18">N14-M14</f>
         <v>1</v>
       </c>
-      <c r="N36" s="4"/>
+      <c r="N36" s="3"/>
       <c r="O36" s="6"/>
       <c r="P36" s="1">
+        <f t="shared" si="4"/>
+        <v>3.640054944640259</v>
+      </c>
+      <c r="Q36" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>3.640054944640259</v>
-      </c>
-      <c r="Q36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S36" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S36" s="1">
-        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="T36" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="V36" s="9">
+      <c r="V36" s="7">
         <f t="shared" si="7"/>
         <v>21</v>
       </c>
-      <c r="W36" s="9">
+      <c r="W36" s="7">
         <f t="shared" si="8"/>
         <v>3.5</v>
       </c>
-      <c r="X36" s="9"/>
+      <c r="X36" s="7"/>
       <c r="Y36" s="8">
         <f>H36-W36</f>
         <v>7.5</v>
@@ -2300,69 +2706,69 @@
         <v>-2.5</v>
       </c>
       <c r="AE36" s="8"/>
-      <c r="AF36" s="9"/>
-      <c r="AG36" s="9"/>
-      <c r="AH36" s="9"/>
-      <c r="AI36" s="9"/>
+      <c r="AF36" s="7"/>
+      <c r="AG36" s="7"/>
+      <c r="AH36" s="7"/>
+      <c r="AI36" s="7"/>
     </row>
     <row r="37" spans="6:35">
       <c r="F37" s="1">
         <v>13</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="2">
         <v>7</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <f t="shared" ref="H37:L37" si="20">I15-H15</f>
         <v>4</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="3">
         <f t="shared" si="20"/>
         <v>4</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="3">
         <f t="shared" si="20"/>
         <v>4</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37" s="3">
         <f t="shared" si="20"/>
         <v>2</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37" s="3">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37" s="3">
         <f t="shared" ref="M37:N37" si="21">N15-M15</f>
         <v>2</v>
       </c>
-      <c r="N37" s="4"/>
+      <c r="N37" s="3"/>
       <c r="O37" s="6"/>
       <c r="P37" s="1">
+        <f t="shared" si="4"/>
+        <v>1.2133516482134197</v>
+      </c>
+      <c r="Q37" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>1.2133516482134197</v>
-      </c>
-      <c r="Q37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S37" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S37" s="1">
-        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="T37" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="V37" s="9">
+      <c r="V37" s="7">
         <f t="shared" si="7"/>
         <v>17</v>
       </c>
-      <c r="W37" s="9">
+      <c r="W37" s="7">
         <f t="shared" si="8"/>
         <v>2.8333333333333335</v>
       </c>
-      <c r="X37" s="9"/>
+      <c r="X37" s="7"/>
       <c r="Y37" s="8">
         <f t="shared" si="10"/>
         <v>1.1666666666666665</v>
@@ -2388,69 +2794,69 @@
         <v>-0.83333333333333348</v>
       </c>
       <c r="AE37" s="8"/>
-      <c r="AF37" s="9"/>
-      <c r="AG37" s="9"/>
-      <c r="AH37" s="9"/>
-      <c r="AI37" s="9"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
     </row>
     <row r="38" spans="6:35">
       <c r="F38" s="1">
         <v>14</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="2">
         <v>7</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <f t="shared" ref="H38:L38" si="22">I16-H16</f>
         <v>5</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="3">
         <f t="shared" si="22"/>
         <v>5</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="3">
         <f t="shared" si="22"/>
         <v>2</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="3">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="3">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38" s="3">
         <f t="shared" ref="M38:N38" si="23">N16-M16</f>
         <v>2</v>
       </c>
-      <c r="N38" s="4"/>
+      <c r="N38" s="3"/>
       <c r="O38" s="6"/>
       <c r="P38" s="1">
+        <f t="shared" si="4"/>
+        <v>1.699673171197595</v>
+      </c>
+      <c r="Q38" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>1.699673171197595</v>
-      </c>
-      <c r="Q38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S38" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S38" s="1">
-        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="T38" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="V38" s="9">
+      <c r="V38" s="7">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="W38" s="9">
+      <c r="W38" s="7">
         <f t="shared" si="8"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="X38" s="9"/>
+      <c r="X38" s="7"/>
       <c r="Y38" s="8">
         <f t="shared" si="10"/>
         <v>2.3333333333333335</v>
@@ -2476,69 +2882,69 @@
         <v>-0.66666666666666652</v>
       </c>
       <c r="AE38" s="8"/>
-      <c r="AF38" s="9"/>
-      <c r="AG38" s="9"/>
-      <c r="AH38" s="9"/>
-      <c r="AI38" s="9"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
+      <c r="AI38" s="7"/>
     </row>
     <row r="39" spans="6:35">
       <c r="F39" s="1">
         <v>15</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="2">
         <v>7</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="3">
         <f t="shared" ref="H39:L39" si="24">I17-H17</f>
         <v>6</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="3">
         <f t="shared" si="24"/>
         <v>2</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="3">
         <f t="shared" si="24"/>
         <v>4</v>
       </c>
-      <c r="K39" s="4">
+      <c r="K39" s="3">
         <f t="shared" si="24"/>
         <v>2</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="3">
         <f t="shared" si="24"/>
         <v>1</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39" s="3">
         <f t="shared" ref="M39:N39" si="25">N17-M17</f>
         <v>20</v>
       </c>
-      <c r="N39" s="4"/>
+      <c r="N39" s="3"/>
       <c r="O39" s="6"/>
       <c r="P39" s="1">
+        <f t="shared" si="4"/>
+        <v>6.5425954754635072</v>
+      </c>
+      <c r="Q39" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>6.5425954754635072</v>
-      </c>
-      <c r="Q39" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S39" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S39" s="1">
-        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="T39" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="V39" s="9">
+      <c r="V39" s="7">
         <f t="shared" si="7"/>
         <v>35</v>
       </c>
-      <c r="W39" s="9">
+      <c r="W39" s="7">
         <f t="shared" si="8"/>
         <v>5.833333333333333</v>
       </c>
-      <c r="X39" s="9"/>
+      <c r="X39" s="7"/>
       <c r="Y39" s="8">
         <f>H39-W39</f>
         <v>0.16666666666666696</v>
@@ -2564,69 +2970,69 @@
         <v>14.166666666666668</v>
       </c>
       <c r="AE39" s="8"/>
-      <c r="AF39" s="9"/>
-      <c r="AG39" s="9"/>
-      <c r="AH39" s="9"/>
-      <c r="AI39" s="9"/>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
     </row>
     <row r="40" spans="6:35">
       <c r="F40" s="1">
         <v>16</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="2">
         <v>7</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <f t="shared" ref="H40:L40" si="26">I18-H18</f>
         <v>6</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="3">
         <f t="shared" si="26"/>
         <v>3</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40" s="3">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
-      <c r="K40" s="4">
+      <c r="K40" s="3">
         <f t="shared" si="26"/>
         <v>1</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="3">
         <f t="shared" si="26"/>
         <v>2</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40" s="3">
         <f t="shared" ref="M40:N40" si="27">N18-M18</f>
         <v>1</v>
       </c>
-      <c r="N40" s="4"/>
+      <c r="N40" s="3"/>
       <c r="O40" s="6"/>
       <c r="P40" s="1">
+        <f t="shared" si="4"/>
+        <v>1.7950549357115013</v>
+      </c>
+      <c r="Q40" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>1.7950549357115013</v>
-      </c>
-      <c r="Q40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S40" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S40" s="1">
-        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="T40" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="V40" s="9">
+      <c r="V40" s="7">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="W40" s="9">
+      <c r="W40" s="7">
         <f t="shared" si="8"/>
         <v>2.3333333333333335</v>
       </c>
-      <c r="X40" s="9"/>
+      <c r="X40" s="7"/>
       <c r="Y40" s="8">
         <f t="shared" si="10"/>
         <v>3.6666666666666665</v>
@@ -2652,69 +3058,69 @@
         <v>-1.3333333333333335</v>
       </c>
       <c r="AE40" s="8"/>
-      <c r="AF40" s="9"/>
-      <c r="AG40" s="9"/>
-      <c r="AH40" s="9"/>
-      <c r="AI40" s="9"/>
+      <c r="AF40" s="7"/>
+      <c r="AG40" s="7"/>
+      <c r="AH40" s="7"/>
+      <c r="AI40" s="7"/>
     </row>
     <row r="41" spans="6:35">
       <c r="F41" s="1">
         <v>17</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="2">
         <v>7</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="3">
         <f t="shared" ref="H41:L41" si="28">I19-H19</f>
         <v>2</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I41" s="3">
         <f t="shared" si="28"/>
         <v>6</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41" s="3">
         <f t="shared" si="28"/>
         <v>2</v>
       </c>
-      <c r="K41" s="4">
+      <c r="K41" s="3">
         <f t="shared" si="28"/>
         <v>2</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="3">
         <f t="shared" si="28"/>
         <v>1</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41" s="3">
         <f t="shared" ref="M41:N41" si="29">N19-M19</f>
         <v>20</v>
       </c>
-      <c r="N41" s="4"/>
+      <c r="N41" s="3"/>
       <c r="O41" s="6"/>
       <c r="P41" s="1">
+        <f t="shared" si="4"/>
+        <v>6.6770752080033766</v>
+      </c>
+      <c r="Q41" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>6.6770752080033766</v>
-      </c>
-      <c r="Q41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S41" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S41" s="1">
-        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="T41" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="V41" s="9">
+      <c r="V41" s="7">
         <f t="shared" si="7"/>
         <v>33</v>
       </c>
-      <c r="W41" s="9">
+      <c r="W41" s="7">
         <f t="shared" si="8"/>
         <v>5.5</v>
       </c>
-      <c r="X41" s="9"/>
+      <c r="X41" s="7"/>
       <c r="Y41" s="8">
         <f t="shared" si="10"/>
         <v>-3.5</v>
@@ -2740,72 +3146,72 @@
         <v>14.5</v>
       </c>
       <c r="AE41" s="8"/>
-      <c r="AF41" s="9"/>
-      <c r="AG41" s="9"/>
-      <c r="AH41" s="9"/>
-      <c r="AI41" s="9"/>
+      <c r="AF41" s="7"/>
+      <c r="AG41" s="7"/>
+      <c r="AH41" s="7"/>
+      <c r="AI41" s="7"/>
     </row>
     <row r="42" spans="6:35">
       <c r="F42" s="1">
         <v>18</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="2">
         <v>8</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42" s="3">
         <f t="shared" ref="H42:L42" si="30">I20-H20</f>
         <v>2</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42" s="3">
         <f t="shared" si="30"/>
         <v>2</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="3">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="3">
         <f t="shared" si="30"/>
         <v>18</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="3">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M42" s="3">
         <f t="shared" ref="M42:N42" si="31">N20-M20</f>
         <v>14</v>
       </c>
-      <c r="N42" s="4">
+      <c r="N42" s="3">
         <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="O42" s="6"/>
       <c r="P42" s="1">
+        <f t="shared" si="4"/>
+        <v>6.6944997222057037</v>
+      </c>
+      <c r="Q42" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>6.6944997222057037</v>
-      </c>
-      <c r="Q42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S42" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S42" s="1">
-        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="T42" s="1">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="V42" s="9">
+      <c r="V42" s="7">
         <f t="shared" si="7"/>
         <v>39</v>
       </c>
-      <c r="W42" s="9">
+      <c r="W42" s="7">
         <f t="shared" si="8"/>
         <v>5.5714285714285712</v>
       </c>
-      <c r="X42" s="9"/>
+      <c r="X42" s="7"/>
       <c r="Y42" s="8">
         <f t="shared" si="10"/>
         <v>-3.5714285714285712</v>
@@ -2834,72 +3240,72 @@
         <f>N42-W42</f>
         <v>-4.5714285714285712</v>
       </c>
-      <c r="AF42" s="9"/>
-      <c r="AG42" s="9"/>
-      <c r="AH42" s="9"/>
-      <c r="AI42" s="9"/>
+      <c r="AF42" s="7"/>
+      <c r="AG42" s="7"/>
+      <c r="AH42" s="7"/>
+      <c r="AI42" s="7"/>
     </row>
     <row r="43" spans="6:35">
       <c r="F43" s="1">
         <v>19</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="2">
         <v>8</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="3">
         <f t="shared" ref="H43:L43" si="32">I21-H21</f>
         <v>3</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="3">
         <f t="shared" si="32"/>
         <v>11</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="3">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
-      <c r="K43" s="4">
+      <c r="K43" s="3">
         <f t="shared" si="32"/>
         <v>2</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="3">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
-      <c r="M43" s="4">
+      <c r="M43" s="3">
         <f t="shared" ref="M43:N43" si="33">N21-M21</f>
         <v>6</v>
       </c>
-      <c r="N43" s="4">
+      <c r="N43" s="3">
         <f>O21-N21</f>
         <v>26</v>
       </c>
       <c r="O43" s="6"/>
       <c r="P43" s="1">
+        <f t="shared" si="4"/>
+        <v>8.3739147941444827</v>
+      </c>
+      <c r="Q43" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>8.3739147941444827</v>
-      </c>
-      <c r="Q43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S43" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S43" s="1">
-        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="T43" s="1">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="V43" s="9">
+      <c r="V43" s="7">
         <f t="shared" si="7"/>
         <v>50</v>
       </c>
-      <c r="W43" s="9">
+      <c r="W43" s="7">
         <f t="shared" si="8"/>
         <v>7.1428571428571432</v>
       </c>
-      <c r="X43" s="9"/>
+      <c r="X43" s="7"/>
       <c r="Y43" s="8">
         <f t="shared" si="10"/>
         <v>-4.1428571428571432</v>
@@ -2928,72 +3334,72 @@
         <f t="shared" ref="AE43:AE44" si="34">N43-W43</f>
         <v>18.857142857142858</v>
       </c>
-      <c r="AF43" s="9"/>
-      <c r="AG43" s="9"/>
-      <c r="AH43" s="9"/>
-      <c r="AI43" s="9"/>
+      <c r="AF43" s="7"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7"/>
     </row>
     <row r="44" spans="6:35">
       <c r="F44" s="1">
         <v>20</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="2">
         <v>8</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="3">
         <f t="shared" ref="H44:L44" si="35">I22-H22</f>
         <v>6</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44" s="3">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44" s="3">
         <f t="shared" si="35"/>
         <v>3</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K44" s="3">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L44" s="3">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="M44" s="4">
+      <c r="M44" s="3">
         <f t="shared" ref="M44:N44" si="36">N22-M22</f>
         <v>2</v>
       </c>
-      <c r="N44" s="4">
+      <c r="N44" s="3">
         <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="O44" s="6"/>
       <c r="P44" s="1">
+        <f t="shared" si="4"/>
+        <v>2.0995626366712954</v>
+      </c>
+      <c r="Q44" s="1" t="b">
         <f t="shared" si="5"/>
-        <v>2.0995626366712954</v>
-      </c>
-      <c r="Q44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S44" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="S44" s="1">
-        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="T44" s="1">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="V44" s="9">
+      <c r="V44" s="7">
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="W44" s="9">
+      <c r="W44" s="7">
         <f>V44/(G44-1)</f>
         <v>2.8571428571428572</v>
       </c>
-      <c r="X44" s="9"/>
+      <c r="X44" s="7"/>
       <c r="Y44" s="8">
         <f>H44-W44</f>
         <v>3.1428571428571428</v>
@@ -3022,48 +3428,48 @@
         <f>N44-W44</f>
         <v>-1.8571428571428572</v>
       </c>
-      <c r="AF44" s="9"/>
-      <c r="AG44" s="9"/>
-      <c r="AH44" s="9"/>
-      <c r="AI44" s="9"/>
+      <c r="AF44" s="7"/>
+      <c r="AG44" s="7"/>
+      <c r="AH44" s="7"/>
+      <c r="AI44" s="7"/>
     </row>
     <row r="45" spans="6:35">
-      <c r="V45" s="9"/>
-      <c r="W45" s="9"/>
-      <c r="X45" s="9"/>
-      <c r="Y45" s="7">
+      <c r="V45" s="7"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="7"/>
+      <c r="Y45" s="9">
         <f>Y26*Y26</f>
         <v>0</v>
       </c>
-      <c r="Z45" s="7">
+      <c r="Z45" s="9">
         <f t="shared" ref="Z45:AE45" si="37">Z26*Z26</f>
         <v>0</v>
       </c>
-      <c r="AA45" s="7">
+      <c r="AA45" s="9">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="AB45" s="7">
+      <c r="AB45" s="9">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="AC45" s="7">
+      <c r="AC45" s="9">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="AD45" s="7">
+      <c r="AD45" s="9">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="AE45" s="7">
+      <c r="AE45" s="9">
         <f t="shared" si="37"/>
         <v>0</v>
       </c>
-      <c r="AF45" s="9">
+      <c r="AF45" s="7">
         <f>SUM(Y45:AE45)</f>
         <v>0</v>
       </c>
-      <c r="AG45" s="9">
+      <c r="AG45" s="7">
         <f>AF45/1</f>
         <v>0</v>
       </c>
@@ -3071,48 +3477,48 @@
         <f>SQRT(AG45)</f>
         <v>0</v>
       </c>
-      <c r="AI45" s="9">
+      <c r="AI45" s="7">
         <f>AH45-P26</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="6:35">
-      <c r="V46" s="9"/>
-      <c r="W46" s="9"/>
-      <c r="X46" s="9"/>
-      <c r="Y46" s="7">
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="7"/>
+      <c r="Y46" s="9">
         <f>Y27*Y27</f>
         <v>0.25</v>
       </c>
-      <c r="Z46" s="7">
+      <c r="Z46" s="9">
         <f t="shared" ref="Y46:AE63" si="38">Z27*Z27</f>
         <v>0.25</v>
       </c>
-      <c r="AA46" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AB46" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AC46" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AD46" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AE46" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF46" s="9">
+      <c r="AA46" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AB46" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AC46" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AD46" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AE46" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF46" s="7">
         <f>SUM(Y46:AE46)</f>
         <v>0.5</v>
       </c>
-      <c r="AG46" s="9">
+      <c r="AG46" s="7">
         <f>AF46/2</f>
         <v>0.25</v>
       </c>
@@ -3120,48 +3526,48 @@
         <f t="shared" ref="AH46:AH63" si="39">SQRT(AG46)</f>
         <v>0.5</v>
       </c>
-      <c r="AI46" s="9">
+      <c r="AI46" s="7">
         <f>AH46-P27</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="6:35">
-      <c r="V47" s="9"/>
-      <c r="W47" s="9"/>
-      <c r="X47" s="9"/>
-      <c r="Y47" s="7">
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="9">
         <f>Y28*Y28</f>
         <v>0</v>
       </c>
-      <c r="Z47" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AA47" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AB47" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AC47" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AD47" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AE47" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF47" s="9">
+      <c r="Z47" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AA47" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AB47" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AC47" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AD47" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AE47" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF47" s="7">
         <f>SUM(Y47:AE47)</f>
         <v>0</v>
       </c>
-      <c r="AG47" s="9">
+      <c r="AG47" s="7">
         <f>AF47/2</f>
         <v>0</v>
       </c>
@@ -3169,48 +3575,48 @@
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AI47" s="9">
+      <c r="AI47" s="7">
         <f t="shared" ref="AI47:AI63" si="40">AH47-P28</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="6:35">
-      <c r="V48" s="9"/>
-      <c r="W48" s="9"/>
-      <c r="X48" s="9"/>
-      <c r="Y48" s="7">
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7"/>
+      <c r="Y48" s="9">
         <f t="shared" si="38"/>
         <v>9</v>
       </c>
-      <c r="Z48" s="7">
+      <c r="Z48" s="9">
         <f>Z29*Z29</f>
         <v>4</v>
       </c>
-      <c r="AA48" s="7">
-        <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="AB48" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AC48" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AD48" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AE48" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF48" s="9">
+      <c r="AA48" s="9">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="AB48" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AC48" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AD48" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AE48" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF48" s="7">
         <f>SUM(Y48:AE48)</f>
         <v>14</v>
       </c>
-      <c r="AG48" s="9">
+      <c r="AG48" s="7">
         <f>AF48/3</f>
         <v>4.666666666666667</v>
       </c>
@@ -3218,48 +3624,48 @@
         <f t="shared" si="39"/>
         <v>2.1602468994692869</v>
       </c>
-      <c r="AI48" s="9">
+      <c r="AI48" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="22:35">
-      <c r="V49" s="9"/>
-      <c r="W49" s="9"/>
-      <c r="X49" s="9"/>
-      <c r="Y49" s="7">
+      <c r="V49" s="7"/>
+      <c r="W49" s="7"/>
+      <c r="X49" s="7"/>
+      <c r="Y49" s="9">
         <f>Y30*Y30</f>
         <v>1.7777777777777777</v>
       </c>
-      <c r="Z49" s="7">
+      <c r="Z49" s="9">
         <f t="shared" ref="Z49:AE49" si="41">Z30*Z30</f>
         <v>0.44444444444444453</v>
       </c>
-      <c r="AA49" s="7">
+      <c r="AA49" s="9">
         <f t="shared" si="41"/>
         <v>0.44444444444444453</v>
       </c>
-      <c r="AB49" s="7">
+      <c r="AB49" s="9">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="AC49" s="7">
+      <c r="AC49" s="9">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="AD49" s="7">
+      <c r="AD49" s="9">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="AE49" s="7">
+      <c r="AE49" s="9">
         <f t="shared" si="41"/>
         <v>0</v>
       </c>
-      <c r="AF49" s="9">
+      <c r="AF49" s="7">
         <f>SUM(Y49:AE49)</f>
         <v>2.666666666666667</v>
       </c>
-      <c r="AG49" s="9">
+      <c r="AG49" s="7">
         <f t="shared" ref="AG49:AG50" si="42">AF49/3</f>
         <v>0.88888888888888895</v>
       </c>
@@ -3267,48 +3673,48 @@
         <f t="shared" si="39"/>
         <v>0.94280904158206336</v>
       </c>
-      <c r="AI49" s="9">
+      <c r="AI49" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="22:35">
-      <c r="V50" s="9"/>
-      <c r="W50" s="9"/>
-      <c r="X50" s="9"/>
-      <c r="Y50" s="7">
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="9">
         <f>Y31*Y31</f>
         <v>0.11111111111111106</v>
       </c>
-      <c r="Z50" s="7">
+      <c r="Z50" s="9">
         <f t="shared" si="38"/>
         <v>0.44444444444444453</v>
       </c>
-      <c r="AA50" s="7">
+      <c r="AA50" s="9">
         <f t="shared" si="38"/>
         <v>0.11111111111111106</v>
       </c>
-      <c r="AB50" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AC50" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AD50" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AE50" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF50" s="9">
+      <c r="AB50" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AC50" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AD50" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AE50" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF50" s="7">
         <f>SUM(Y50:AE50)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="AG50" s="9">
+      <c r="AG50" s="7">
         <f t="shared" si="42"/>
         <v>0.22222222222222221</v>
       </c>
@@ -3316,48 +3722,48 @@
         <f t="shared" si="39"/>
         <v>0.47140452079103168</v>
       </c>
-      <c r="AI50" s="9">
+      <c r="AI50" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="22:35">
-      <c r="V51" s="9"/>
-      <c r="W51" s="9"/>
-      <c r="X51" s="9"/>
-      <c r="Y51" s="7">
+      <c r="V51" s="7"/>
+      <c r="W51" s="7"/>
+      <c r="X51" s="7"/>
+      <c r="Y51" s="9">
         <f>Y32*Y32</f>
         <v>3.0625</v>
       </c>
-      <c r="Z51" s="7">
+      <c r="Z51" s="9">
         <f t="shared" ref="Z51:AE51" si="43">Z32*Z32</f>
         <v>6.25E-2</v>
       </c>
-      <c r="AA51" s="7">
+      <c r="AA51" s="9">
         <f t="shared" si="43"/>
         <v>1.5625</v>
       </c>
-      <c r="AB51" s="7">
+      <c r="AB51" s="9">
         <f t="shared" si="43"/>
         <v>6.25E-2</v>
       </c>
-      <c r="AC51" s="7">
+      <c r="AC51" s="9">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AD51" s="7">
+      <c r="AD51" s="9">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AE51" s="7">
+      <c r="AE51" s="9">
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AF51" s="9">
+      <c r="AF51" s="7">
         <f>SUM(Y51:AE51)</f>
         <v>4.75</v>
       </c>
-      <c r="AG51" s="9">
+      <c r="AG51" s="7">
         <f>AF51/4</f>
         <v>1.1875</v>
       </c>
@@ -3365,48 +3771,48 @@
         <f t="shared" si="39"/>
         <v>1.0897247358851685</v>
       </c>
-      <c r="AI51" s="9">
+      <c r="AI51" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="22:35">
-      <c r="V52" s="9"/>
-      <c r="W52" s="9"/>
-      <c r="X52" s="9"/>
-      <c r="Y52" s="7">
+      <c r="V52" s="7"/>
+      <c r="W52" s="7"/>
+      <c r="X52" s="7"/>
+      <c r="Y52" s="9">
         <f t="shared" si="38"/>
         <v>1.9599999999999997</v>
       </c>
-      <c r="Z52" s="7">
+      <c r="Z52" s="9">
         <f t="shared" si="38"/>
         <v>1.9599999999999997</v>
       </c>
-      <c r="AA52" s="7">
+      <c r="AA52" s="9">
         <f t="shared" si="38"/>
         <v>0.3600000000000001</v>
       </c>
-      <c r="AB52" s="7">
+      <c r="AB52" s="9">
         <f t="shared" si="38"/>
         <v>2.5600000000000005</v>
       </c>
-      <c r="AC52" s="7">
+      <c r="AC52" s="9">
         <f t="shared" si="38"/>
         <v>0.3600000000000001</v>
       </c>
-      <c r="AD52" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AE52" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF52" s="9">
+      <c r="AD52" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AE52" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF52" s="7">
         <f>SUM(Y52:AE52)</f>
         <v>7.2</v>
       </c>
-      <c r="AG52" s="9">
+      <c r="AG52" s="7">
         <f>AF52/5</f>
         <v>1.44</v>
       </c>
@@ -3414,48 +3820,48 @@
         <f t="shared" si="39"/>
         <v>1.2</v>
       </c>
-      <c r="AI52" s="9">
+      <c r="AI52" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="22:35">
-      <c r="V53" s="9"/>
-      <c r="W53" s="9"/>
-      <c r="X53" s="9"/>
-      <c r="Y53" s="7">
+      <c r="V53" s="7"/>
+      <c r="W53" s="7"/>
+      <c r="X53" s="7"/>
+      <c r="Y53" s="9">
         <f t="shared" si="38"/>
         <v>4.000000000000007E-2</v>
       </c>
-      <c r="Z53" s="7">
+      <c r="Z53" s="9">
         <f t="shared" si="38"/>
         <v>7.839999999999999</v>
       </c>
-      <c r="AA53" s="7">
+      <c r="AA53" s="9">
         <f t="shared" si="38"/>
         <v>1.4400000000000004</v>
       </c>
-      <c r="AB53" s="7">
+      <c r="AB53" s="9">
         <f t="shared" si="38"/>
         <v>4.000000000000007E-2</v>
       </c>
-      <c r="AC53" s="7">
+      <c r="AC53" s="9">
         <f t="shared" si="38"/>
         <v>1.4400000000000004</v>
       </c>
-      <c r="AD53" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AE53" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF53" s="9">
+      <c r="AD53" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AE53" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF53" s="7">
         <f>SUM(Y53:AE53)</f>
         <v>10.8</v>
       </c>
-      <c r="AG53" s="9">
+      <c r="AG53" s="7">
         <f>AF53/5</f>
         <v>2.16</v>
       </c>
@@ -3463,48 +3869,48 @@
         <f t="shared" si="39"/>
         <v>1.4696938456699069</v>
       </c>
-      <c r="AI53" s="9">
+      <c r="AI53" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="22:35">
-      <c r="V54" s="9"/>
-      <c r="W54" s="9"/>
-      <c r="X54" s="9"/>
-      <c r="Y54" s="7">
+      <c r="V54" s="7"/>
+      <c r="W54" s="7"/>
+      <c r="X54" s="7"/>
+      <c r="Y54" s="9">
         <f t="shared" si="38"/>
         <v>34.027777777777786</v>
       </c>
-      <c r="Z54" s="7">
+      <c r="Z54" s="9">
         <f t="shared" si="38"/>
         <v>1.3611111111111107</v>
       </c>
-      <c r="AA54" s="7">
+      <c r="AA54" s="9">
         <f t="shared" si="38"/>
         <v>4.6944444444444438</v>
       </c>
-      <c r="AB54" s="7">
+      <c r="AB54" s="9">
         <f t="shared" si="38"/>
         <v>0.69444444444444464</v>
       </c>
-      <c r="AC54" s="7">
+      <c r="AC54" s="9">
         <f t="shared" si="38"/>
         <v>4.6944444444444438</v>
       </c>
-      <c r="AD54" s="7">
+      <c r="AD54" s="9">
         <f t="shared" si="38"/>
         <v>1.3611111111111107</v>
       </c>
-      <c r="AE54" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF54" s="9">
+      <c r="AE54" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF54" s="7">
         <f>SUM(Y54:AE54)</f>
         <v>46.833333333333343</v>
       </c>
-      <c r="AG54" s="9">
+      <c r="AG54" s="7">
         <f>AF54/6</f>
         <v>7.8055555555555571</v>
       </c>
@@ -3512,48 +3918,48 @@
         <f t="shared" si="39"/>
         <v>2.793842435706702</v>
       </c>
-      <c r="AI54" s="9">
+      <c r="AI54" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="22:35">
-      <c r="V55" s="9"/>
-      <c r="W55" s="9"/>
-      <c r="X55" s="9"/>
-      <c r="Y55" s="7">
+      <c r="V55" s="7"/>
+      <c r="W55" s="7"/>
+      <c r="X55" s="7"/>
+      <c r="Y55" s="9">
         <f t="shared" si="38"/>
         <v>56.25</v>
       </c>
-      <c r="Z55" s="7">
+      <c r="Z55" s="9">
         <f t="shared" si="38"/>
         <v>6.25</v>
       </c>
-      <c r="AA55" s="7">
+      <c r="AA55" s="9">
         <f t="shared" si="38"/>
         <v>2.25</v>
       </c>
-      <c r="AB55" s="7">
+      <c r="AB55" s="9">
         <f t="shared" si="38"/>
         <v>6.25</v>
       </c>
-      <c r="AC55" s="7">
+      <c r="AC55" s="9">
         <f t="shared" si="38"/>
         <v>2.25</v>
       </c>
-      <c r="AD55" s="7">
+      <c r="AD55" s="9">
         <f t="shared" si="38"/>
         <v>6.25</v>
       </c>
-      <c r="AE55" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF55" s="9">
+      <c r="AE55" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF55" s="7">
         <f>SUM(Y55:AE55)</f>
         <v>79.5</v>
       </c>
-      <c r="AG55" s="9">
+      <c r="AG55" s="7">
         <f t="shared" ref="AG55:AG60" si="44">AF55/6</f>
         <v>13.25</v>
       </c>
@@ -3561,48 +3967,48 @@
         <f t="shared" si="39"/>
         <v>3.640054944640259</v>
       </c>
-      <c r="AI55" s="9">
+      <c r="AI55" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="22:35">
-      <c r="V56" s="9"/>
-      <c r="W56" s="9"/>
-      <c r="X56" s="9"/>
-      <c r="Y56" s="7">
+      <c r="V56" s="7"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="7"/>
+      <c r="Y56" s="9">
         <f t="shared" si="38"/>
         <v>1.3611111111111107</v>
       </c>
-      <c r="Z56" s="7">
+      <c r="Z56" s="9">
         <f t="shared" si="38"/>
         <v>1.3611111111111107</v>
       </c>
-      <c r="AA56" s="7">
+      <c r="AA56" s="9">
         <f t="shared" si="38"/>
         <v>1.3611111111111107</v>
       </c>
-      <c r="AB56" s="7">
+      <c r="AB56" s="9">
         <f t="shared" si="38"/>
         <v>0.69444444444444464</v>
       </c>
-      <c r="AC56" s="7">
+      <c r="AC56" s="9">
         <f t="shared" si="38"/>
         <v>3.3611111111111116</v>
       </c>
-      <c r="AD56" s="7">
+      <c r="AD56" s="9">
         <f t="shared" si="38"/>
         <v>0.69444444444444464</v>
       </c>
-      <c r="AE56" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF56" s="9">
+      <c r="AE56" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF56" s="7">
         <f>SUM(Y56:AE56)</f>
         <v>8.8333333333333339</v>
       </c>
-      <c r="AG56" s="9">
+      <c r="AG56" s="7">
         <f t="shared" si="44"/>
         <v>1.4722222222222223</v>
       </c>
@@ -3610,48 +4016,48 @@
         <f t="shared" si="39"/>
         <v>1.2133516482134197</v>
       </c>
-      <c r="AI56" s="9">
+      <c r="AI56" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="22:35">
-      <c r="V57" s="9"/>
-      <c r="W57" s="9"/>
-      <c r="X57" s="9"/>
-      <c r="Y57" s="7">
+      <c r="V57" s="7"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="7"/>
+      <c r="Y57" s="9">
         <f t="shared" si="38"/>
         <v>5.4444444444444455</v>
       </c>
-      <c r="Z57" s="7">
+      <c r="Z57" s="9">
         <f t="shared" si="38"/>
         <v>5.4444444444444455</v>
       </c>
-      <c r="AA57" s="7">
+      <c r="AA57" s="9">
         <f t="shared" si="38"/>
         <v>0.44444444444444425</v>
       </c>
-      <c r="AB57" s="7">
+      <c r="AB57" s="9">
         <f t="shared" si="38"/>
         <v>2.7777777777777772</v>
       </c>
-      <c r="AC57" s="7">
+      <c r="AC57" s="9">
         <f t="shared" si="38"/>
         <v>2.7777777777777772</v>
       </c>
-      <c r="AD57" s="7">
+      <c r="AD57" s="9">
         <f t="shared" si="38"/>
         <v>0.44444444444444425</v>
       </c>
-      <c r="AE57" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF57" s="9">
+      <c r="AE57" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF57" s="7">
         <f>SUM(Y57:AE57)</f>
         <v>17.333333333333332</v>
       </c>
-      <c r="AG57" s="9">
+      <c r="AG57" s="7">
         <f t="shared" si="44"/>
         <v>2.8888888888888888</v>
       </c>
@@ -3659,48 +4065,48 @@
         <f t="shared" si="39"/>
         <v>1.699673171197595</v>
       </c>
-      <c r="AI57" s="9">
+      <c r="AI57" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="22:35">
-      <c r="V58" s="9"/>
-      <c r="W58" s="9"/>
-      <c r="X58" s="9"/>
-      <c r="Y58" s="7">
+      <c r="V58" s="7"/>
+      <c r="W58" s="7"/>
+      <c r="X58" s="7"/>
+      <c r="Y58" s="9">
         <f t="shared" si="38"/>
         <v>2.7777777777777877E-2</v>
       </c>
-      <c r="Z58" s="7">
+      <c r="Z58" s="9">
         <f t="shared" si="38"/>
         <v>14.694444444444443</v>
       </c>
-      <c r="AA58" s="7">
+      <c r="AA58" s="9">
         <f t="shared" si="38"/>
         <v>3.3611111111111098</v>
       </c>
-      <c r="AB58" s="7">
+      <c r="AB58" s="9">
         <f t="shared" si="38"/>
         <v>14.694444444444443</v>
       </c>
-      <c r="AC58" s="7">
+      <c r="AC58" s="9">
         <f t="shared" si="38"/>
         <v>23.361111111111107</v>
       </c>
-      <c r="AD58" s="7">
+      <c r="AD58" s="9">
         <f t="shared" si="38"/>
         <v>200.69444444444449</v>
       </c>
-      <c r="AE58" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF58" s="9">
+      <c r="AE58" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF58" s="7">
         <f>SUM(Y58:AE58)</f>
         <v>256.83333333333337</v>
       </c>
-      <c r="AG58" s="9">
+      <c r="AG58" s="7">
         <f t="shared" si="44"/>
         <v>42.805555555555564</v>
       </c>
@@ -3708,48 +4114,48 @@
         <f t="shared" si="39"/>
         <v>6.5425954754635081</v>
       </c>
-      <c r="AI58" s="9">
+      <c r="AI58" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="22:35">
-      <c r="V59" s="9"/>
-      <c r="W59" s="9"/>
-      <c r="X59" s="9"/>
-      <c r="Y59" s="7">
+      <c r="V59" s="7"/>
+      <c r="W59" s="7"/>
+      <c r="X59" s="7"/>
+      <c r="Y59" s="9">
         <f t="shared" si="38"/>
         <v>13.444444444444443</v>
       </c>
-      <c r="Z59" s="7">
+      <c r="Z59" s="9">
         <f t="shared" si="38"/>
         <v>0.44444444444444425</v>
       </c>
-      <c r="AA59" s="7">
+      <c r="AA59" s="9">
         <f t="shared" si="38"/>
         <v>1.7777777777777781</v>
       </c>
-      <c r="AB59" s="7">
+      <c r="AB59" s="9">
         <f t="shared" si="38"/>
         <v>1.7777777777777781</v>
       </c>
-      <c r="AC59" s="7">
+      <c r="AC59" s="9">
         <f t="shared" si="38"/>
         <v>0.11111111111111122</v>
       </c>
-      <c r="AD59" s="7">
+      <c r="AD59" s="9">
         <f t="shared" si="38"/>
         <v>1.7777777777777781</v>
       </c>
-      <c r="AE59" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF59" s="9">
+      <c r="AE59" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF59" s="7">
         <f>SUM(Y59:AE59)</f>
         <v>19.333333333333332</v>
       </c>
-      <c r="AG59" s="9">
+      <c r="AG59" s="7">
         <f t="shared" si="44"/>
         <v>3.2222222222222219</v>
       </c>
@@ -3757,48 +4163,48 @@
         <f t="shared" si="39"/>
         <v>1.7950549357115013</v>
       </c>
-      <c r="AI59" s="9">
+      <c r="AI59" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="22:35">
-      <c r="V60" s="9"/>
-      <c r="W60" s="9"/>
-      <c r="X60" s="9"/>
-      <c r="Y60" s="7">
+      <c r="V60" s="7"/>
+      <c r="W60" s="7"/>
+      <c r="X60" s="7"/>
+      <c r="Y60" s="9">
         <f t="shared" si="38"/>
         <v>12.25</v>
       </c>
-      <c r="Z60" s="7">
+      <c r="Z60" s="9">
         <f t="shared" si="38"/>
         <v>0.25</v>
       </c>
-      <c r="AA60" s="7">
+      <c r="AA60" s="9">
         <f t="shared" si="38"/>
         <v>12.25</v>
       </c>
-      <c r="AB60" s="7">
+      <c r="AB60" s="9">
         <f t="shared" si="38"/>
         <v>12.25</v>
       </c>
-      <c r="AC60" s="7">
+      <c r="AC60" s="9">
         <f t="shared" si="38"/>
         <v>20.25</v>
       </c>
-      <c r="AD60" s="7">
+      <c r="AD60" s="9">
         <f t="shared" si="38"/>
         <v>210.25</v>
       </c>
-      <c r="AE60" s="7">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="AF60" s="9">
+      <c r="AE60" s="9">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AF60" s="7">
         <f>SUM(Y60:AE60)</f>
         <v>267.5</v>
       </c>
-      <c r="AG60" s="9">
+      <c r="AG60" s="7">
         <f t="shared" si="44"/>
         <v>44.583333333333336</v>
       </c>
@@ -3806,48 +4212,48 @@
         <f t="shared" si="39"/>
         <v>6.6770752080033766</v>
       </c>
-      <c r="AI60" s="9">
+      <c r="AI60" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="22:35">
-      <c r="V61" s="9"/>
-      <c r="W61" s="9"/>
-      <c r="X61" s="9"/>
-      <c r="Y61" s="7">
+      <c r="V61" s="7"/>
+      <c r="W61" s="7"/>
+      <c r="X61" s="7"/>
+      <c r="Y61" s="9">
         <f t="shared" si="38"/>
         <v>12.755102040816325</v>
       </c>
-      <c r="Z61" s="7">
+      <c r="Z61" s="9">
         <f t="shared" si="38"/>
         <v>12.755102040816325</v>
       </c>
-      <c r="AA61" s="7">
+      <c r="AA61" s="9">
         <f t="shared" si="38"/>
         <v>20.897959183673468</v>
       </c>
-      <c r="AB61" s="7">
+      <c r="AB61" s="9">
         <f t="shared" si="38"/>
         <v>154.46938775510205</v>
       </c>
-      <c r="AC61" s="7">
+      <c r="AC61" s="9">
         <f t="shared" si="38"/>
         <v>20.897959183673468</v>
       </c>
-      <c r="AD61" s="7">
+      <c r="AD61" s="9">
         <f t="shared" si="38"/>
         <v>71.040816326530617</v>
       </c>
-      <c r="AE61" s="7">
+      <c r="AE61" s="9">
         <f t="shared" si="38"/>
         <v>20.897959183673468</v>
       </c>
-      <c r="AF61" s="9">
+      <c r="AF61" s="7">
         <f>SUM(Y61:AE61)</f>
         <v>313.71428571428572</v>
       </c>
-      <c r="AG61" s="9">
+      <c r="AG61" s="7">
         <f>AF61/7</f>
         <v>44.816326530612244</v>
       </c>
@@ -3855,48 +4261,48 @@
         <f t="shared" si="39"/>
         <v>6.6944997222057037</v>
       </c>
-      <c r="AI61" s="9">
+      <c r="AI61" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="22:35">
-      <c r="V62" s="9"/>
-      <c r="W62" s="9"/>
-      <c r="X62" s="9"/>
-      <c r="Y62" s="7">
+      <c r="V62" s="7"/>
+      <c r="W62" s="7"/>
+      <c r="X62" s="7"/>
+      <c r="Y62" s="9">
         <f t="shared" si="38"/>
         <v>17.163265306122451</v>
       </c>
-      <c r="Z62" s="7">
+      <c r="Z62" s="9">
         <f t="shared" si="38"/>
         <v>14.877551020408161</v>
       </c>
-      <c r="AA62" s="7">
+      <c r="AA62" s="9">
         <f t="shared" si="38"/>
         <v>37.734693877551024</v>
       </c>
-      <c r="AB62" s="7">
+      <c r="AB62" s="9">
         <f t="shared" si="38"/>
         <v>26.448979591836739</v>
       </c>
-      <c r="AC62" s="7">
+      <c r="AC62" s="9">
         <f t="shared" si="38"/>
         <v>37.734693877551024</v>
       </c>
-      <c r="AD62" s="7">
+      <c r="AD62" s="9">
         <f t="shared" si="38"/>
         <v>1.3061224489795926</v>
       </c>
-      <c r="AE62" s="7">
+      <c r="AE62" s="9">
         <f>AE43*AE43</f>
         <v>355.59183673469391</v>
       </c>
-      <c r="AF62" s="9">
+      <c r="AF62" s="7">
         <f>SUM(Y62:AE62)</f>
         <v>490.85714285714289</v>
       </c>
-      <c r="AG62" s="9">
+      <c r="AG62" s="7">
         <f t="shared" ref="AG62:AG63" si="45">AF62/7</f>
         <v>70.122448979591837</v>
       </c>
@@ -3904,48 +4310,48 @@
         <f t="shared" si="39"/>
         <v>8.3739147941444827</v>
       </c>
-      <c r="AI62" s="9">
+      <c r="AI62" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="22:35">
-      <c r="V63" s="9"/>
-      <c r="W63" s="9"/>
-      <c r="X63" s="9"/>
-      <c r="Y63" s="7">
+      <c r="V63" s="7"/>
+      <c r="W63" s="7"/>
+      <c r="X63" s="7"/>
+      <c r="Y63" s="9">
         <f t="shared" si="38"/>
         <v>9.8775510204081627</v>
       </c>
-      <c r="Z63" s="7">
+      <c r="Z63" s="9">
         <f t="shared" si="38"/>
         <v>9.8775510204081627</v>
       </c>
-      <c r="AA63" s="7">
+      <c r="AA63" s="9">
         <f t="shared" si="38"/>
         <v>2.0408163265306103E-2</v>
       </c>
-      <c r="AB63" s="7">
+      <c r="AB63" s="9">
         <f t="shared" si="38"/>
         <v>3.4489795918367347</v>
       </c>
-      <c r="AC63" s="7">
+      <c r="AC63" s="9">
         <f t="shared" si="38"/>
         <v>3.4489795918367347</v>
       </c>
-      <c r="AD63" s="7">
+      <c r="AD63" s="9">
         <f t="shared" si="38"/>
         <v>0.73469387755102056</v>
       </c>
-      <c r="AE63" s="7">
+      <c r="AE63" s="9">
         <f t="shared" si="38"/>
         <v>3.4489795918367347</v>
       </c>
-      <c r="AF63" s="9">
+      <c r="AF63" s="7">
         <f>SUM(Y63:AE63)</f>
         <v>30.857142857142858</v>
       </c>
-      <c r="AG63" s="9">
+      <c r="AG63" s="7">
         <f t="shared" si="45"/>
         <v>4.4081632653061229</v>
       </c>
@@ -3953,12 +4359,36 @@
         <f t="shared" si="39"/>
         <v>2.0995626366712958</v>
       </c>
-      <c r="AI63" s="9">
+      <c r="AI63" s="7">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="Y11:Z11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>